<commit_message>
refine register, login apply job with storage state,
</commit_message>
<xml_diff>
--- a/accountData.xlsx
+++ b/accountData.xlsx
@@ -412,10 +412,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>ypvyak88yy@gmail.com</v>
+        <v>1qmh5a3697@gmail.com</v>
       </c>
       <c r="B2" t="str">
-        <v xml:space="preserve">Testing@123 </v>
+        <v>Testing@123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>